<commit_message>
Some tests, plus adjustments to Rui's flow code, plus support functions to tell us if a flow overtops a levee
</commit_message>
<xml_diff>
--- a/HW/HW2/ExampleSpreadsheet.xlsx
+++ b/HW/HW2/ExampleSpreadsheet.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20325" windowHeight="9630"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20325" windowHeight="9630" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="12">
   <si>
     <t>Stage 200</t>
   </si>
@@ -51,6 +52,15 @@
   </si>
   <si>
     <t>EAD+r*40*[200f*]</t>
+  </si>
+  <si>
+    <t>Height</t>
+  </si>
+  <si>
+    <t>Mean Flow</t>
+  </si>
+  <si>
+    <t>Flow SD</t>
   </si>
 </sst>
 </file>
@@ -385,8 +395,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -981,4 +991,517 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:R33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="I3">
+        <v>3</v>
+      </c>
+      <c r="J3">
+        <v>4</v>
+      </c>
+      <c r="K3">
+        <v>5</v>
+      </c>
+      <c r="L3">
+        <v>6</v>
+      </c>
+      <c r="M3">
+        <v>7</v>
+      </c>
+      <c r="N3">
+        <v>8</v>
+      </c>
+      <c r="O3">
+        <v>9</v>
+      </c>
+      <c r="P3">
+        <v>10</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>6</v>
+      </c>
+      <c r="R3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>10</v>
+      </c>
+      <c r="E4">
+        <v>-1</v>
+      </c>
+      <c r="F4">
+        <v>999</v>
+      </c>
+      <c r="G4">
+        <v>900</v>
+      </c>
+      <c r="H4">
+        <v>800</v>
+      </c>
+      <c r="I4">
+        <v>650</v>
+      </c>
+      <c r="J4">
+        <v>665</v>
+      </c>
+      <c r="K4">
+        <v>700</v>
+      </c>
+      <c r="L4">
+        <v>750</v>
+      </c>
+      <c r="M4">
+        <v>800</v>
+      </c>
+      <c r="N4">
+        <v>900</v>
+      </c>
+      <c r="O4">
+        <v>1000</v>
+      </c>
+      <c r="P4">
+        <v>1010</v>
+      </c>
+      <c r="Q4">
+        <v>3</v>
+      </c>
+      <c r="R4">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>20</v>
+      </c>
+      <c r="E5">
+        <v>-1</v>
+      </c>
+      <c r="F5">
+        <f>F4+100</f>
+        <v>1099</v>
+      </c>
+      <c r="G5">
+        <f t="shared" ref="G5:P5" si="0">G4+100</f>
+        <v>1000</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>900</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>750</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>765</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="0"/>
+        <v>800</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="0"/>
+        <v>850</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="0"/>
+        <v>900</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="0"/>
+        <v>1100</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="0"/>
+        <v>1110</v>
+      </c>
+      <c r="Q5">
+        <v>3</v>
+      </c>
+      <c r="R5">
+        <f>MIN(F5:P5)</f>
+        <v>750</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>30</v>
+      </c>
+      <c r="E6">
+        <v>-1</v>
+      </c>
+      <c r="Q6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>40</v>
+      </c>
+      <c r="E7">
+        <v>-1</v>
+      </c>
+      <c r="Q7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>50</v>
+      </c>
+      <c r="E8">
+        <v>-1</v>
+      </c>
+      <c r="Q8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>10</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>20</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="P10" s="1"/>
+      <c r="Q10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>30</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>40</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>50</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>10</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>20</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>30</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>40</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>50</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+      <c r="Q19">
+        <v>0</v>
+      </c>
+      <c r="R19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C24">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C26">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C27">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C28">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C29">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C30">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C31">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C32">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C33">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>